<commit_message>
Small edits in texts, user acts saving fixed
</commit_message>
<xml_diff>
--- a/WebAppForMORecSys/tnorm.xlsx
+++ b/WebAppForMORecSys/tnorm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\patri\source\repos\WebAppForMORecSys\WebAppForMORecSys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D381F6-EE9F-4C6F-A247-4DBC31C43FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84300037-AB08-4333-8A77-C77BEC651057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E0EA0AA2-A36A-4DE3-885E-0C39FAEA5C10}"/>
   </bookViews>
@@ -429,7 +429,7 @@
   <dimension ref="A1:L106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,7 +437,7 @@
     <col min="2" max="3" width="8.88671875" style="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.21875" customWidth="1"/>
     <col min="8" max="8" width="18.88671875" customWidth="1"/>
     <col min="9" max="9" width="5.44140625" customWidth="1"/>
@@ -499,7 +499,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="1">
-        <f>MAX(MAX(D2+B2 -1,0) + C2 - 1,0)</f>
+        <f t="shared" ref="E2:E45" si="0">MAX(MAX(D2+(1.2*B2) -1,0) + (0.8*C2) - 1,0)</f>
         <v>0</v>
       </c>
       <c r="F2" s="1">
@@ -523,11 +523,11 @@
         <v>0</v>
       </c>
       <c r="K2" t="b">
-        <f t="shared" ref="K2:K33" si="0">IF(A2 &lt; 15, AND((B2 &gt;= 1),(C2 &gt;=2/3)), IF(A2 &lt; 30, AND((B2 &gt;= 2/3),(C2&gt;=1/2)),  AND((B2 &gt;= 1/3),(C2&gt;=1/5))))</f>
+        <f t="shared" ref="K2:K33" si="1">IF(A2 &lt; 15, AND((B2 &gt;= 1),(C2 &gt;=2/3)), IF(A2 &lt; 30, AND((B2 &gt;= 2/3),(C2&gt;=1/2)),  AND((B2 &gt;= 1/3),(C2&gt;=1/5))))</f>
         <v>0</v>
       </c>
       <c r="L2" t="b">
-        <f>NOT(J2 = K2)</f>
+        <f>NOT(H2 = K2)</f>
         <v>0</v>
       </c>
     </row>
@@ -543,11 +543,11 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" si="1">MIN(A3,30)/30</f>
+        <f t="shared" ref="D3:D66" si="2">MIN(A3,30)/30</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E66" si="2">MAX(MAX(D3+B3 -1,0) + C3 - 1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F3" s="1">
@@ -571,11 +571,11 @@
         <v>0</v>
       </c>
       <c r="K3" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L3" t="b">
-        <f t="shared" ref="L3:L66" si="8">NOT(J3 = K3)</f>
+        <f t="shared" ref="L3:L66" si="8">NOT(H3 = K3)</f>
         <v>0</v>
       </c>
     </row>
@@ -591,35 +591,35 @@
         <v>0</v>
       </c>
       <c r="D4">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K4" t="b">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I4" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J4" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K4" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4" t="b">
@@ -638,35 +638,35 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H5" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I5" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J5" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K5" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" t="b">
@@ -685,35 +685,35 @@
         <v>0</v>
       </c>
       <c r="D6">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H6" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I6" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J6" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K6" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L6" t="b">
@@ -732,35 +732,35 @@
         <v>0</v>
       </c>
       <c r="D7">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H7" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I7" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J7" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K7" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L7" t="b">
@@ -780,35 +780,35 @@
         <v>0</v>
       </c>
       <c r="D8">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H8" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I8" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J8" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K8" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L8" t="b">
@@ -828,35 +828,35 @@
         <v>0</v>
       </c>
       <c r="D9">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J9" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K9" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L9" t="b">
@@ -875,35 +875,35 @@
         <v>0</v>
       </c>
       <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I10" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J10" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K10" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L10" t="b">
@@ -922,35 +922,35 @@
         <v>0</v>
       </c>
       <c r="D11">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H11" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I11" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J11" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K11" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L11" t="b">
@@ -969,35 +969,35 @@
         <v>0</v>
       </c>
       <c r="D12">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H12" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I12" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J12" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K12" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L12" t="b">
@@ -1017,35 +1017,35 @@
         <v>0</v>
       </c>
       <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H13" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I13" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J13" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K13" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L13" t="b">
@@ -1065,35 +1065,35 @@
         <v>0</v>
       </c>
       <c r="D14">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H14" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I14" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K14" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L14" t="b">
@@ -1112,35 +1112,35 @@
         <v>0</v>
       </c>
       <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H15" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I15" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J15" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L15" t="b">
@@ -1159,35 +1159,35 @@
         <v>0</v>
       </c>
       <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H16" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I16" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J16" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K16" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L16" t="b">
@@ -1206,35 +1206,35 @@
         <v>0</v>
       </c>
       <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H17" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I17" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J17" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K17" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L17" t="b">
@@ -1254,35 +1254,35 @@
         <v>0</v>
       </c>
       <c r="D18">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I18" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J18" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K18" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L18" t="b">
@@ -1302,35 +1302,35 @@
         <v>0</v>
       </c>
       <c r="D19">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I19" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J19" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K19" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L19" t="b">
@@ -1349,35 +1349,35 @@
         <v>0</v>
       </c>
       <c r="D20">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H20" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I20" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J20" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K20" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L20" t="b">
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>25</v>
       </c>
@@ -1396,40 +1396,40 @@
         <v>0</v>
       </c>
       <c r="D21">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333215E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H21" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I21" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J21" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K21" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L21" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -1443,35 +1443,35 @@
         <v>0</v>
       </c>
       <c r="D22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H22" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I22" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J22" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K22" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L22" t="b">
@@ -1491,35 +1491,35 @@
         <v>0</v>
       </c>
       <c r="D23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H23" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I23" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J23" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K23" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L23" t="b">
@@ -1539,35 +1539,35 @@
         <v>0</v>
       </c>
       <c r="D24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H24" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I24" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J24" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K24" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L24" t="b">
@@ -1586,35 +1586,35 @@
         <v>0</v>
       </c>
       <c r="D25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H25" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I25" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J25" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K25" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L25" t="b">
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>30</v>
       </c>
@@ -1633,40 +1633,40 @@
         <v>0</v>
       </c>
       <c r="D26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K26" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H26" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I26" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J26" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K26" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L26" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -1681,35 +1681,35 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D27">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I27" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J27" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K27" t="b">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H27" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I27" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J27" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K27" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L27" t="b">
@@ -1730,35 +1730,35 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D28">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="H28" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J28" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K28" t="b">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="4"/>
-        <v>2.222222222222222E-2</v>
-      </c>
-      <c r="H28" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I28" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J28" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K28" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L28" t="b">
@@ -1779,35 +1779,35 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D29">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>6.6666666666666652E-2</v>
+      </c>
+      <c r="H29" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K29" t="b">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E29" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="4"/>
-        <v>6.6666666666666652E-2</v>
-      </c>
-      <c r="H29" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I29" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J29" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K29" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L29" t="b">
@@ -1827,35 +1827,35 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D30">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="4"/>
+        <v>8.8888888888888878E-2</v>
+      </c>
+      <c r="H30" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K30" t="b">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E30" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="4"/>
-        <v>8.8888888888888878E-2</v>
-      </c>
-      <c r="H30" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I30" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J30" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K30" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L30" t="b">
@@ -1875,35 +1875,35 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D31">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="H31" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E31" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="1">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="H31" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I31" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="J31" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K31" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L31" t="b">
@@ -1923,35 +1923,35 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D32">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E32" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H32" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I32" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J32" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K32" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L32" t="b">
@@ -1972,35 +1972,35 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D33">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H33" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="4"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="H33" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I33" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J33" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K33" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L33" t="b">
@@ -2021,11 +2021,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F34" s="1">
@@ -2069,11 +2069,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F35" s="1">
@@ -2117,11 +2117,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F36" s="1">
@@ -2165,11 +2165,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F37" s="1">
@@ -2214,11 +2214,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F38" s="1">
@@ -2263,11 +2263,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F39" s="1">
@@ -2311,11 +2311,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F40" s="1">
@@ -2347,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>20</v>
       </c>
@@ -2359,12 +2359,12 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.1333333333333333</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="3"/>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="H41" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="b">
         <f t="shared" si="6"/>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="L41" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -2407,11 +2407,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F42" s="1">
@@ -2456,11 +2456,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F43" s="1">
@@ -2505,11 +2505,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F44" s="1">
@@ -2541,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>25</v>
       </c>
@@ -2553,12 +2553,12 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000053E-2</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="3"/>
@@ -2570,7 +2570,7 @@
       </c>
       <c r="H45" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" t="b">
         <f t="shared" si="6"/>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="L45" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2601,12 +2601,12 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="2"/>
-        <v>0.16666666666666674</v>
+        <f>MAX(MAX(D46+(1.2*B46) -1,0) + (0.8*C46) - 1,0)</f>
+        <v>0.29999999999999982</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="3"/>
@@ -2649,11 +2649,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E47:E101" si="11">MAX(MAX(D47+(1.2*B47) -1,0) + (0.8*C47) - 1,0)</f>
         <v>0</v>
       </c>
       <c r="F47" s="1">
@@ -2698,11 +2698,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F48" s="1">
@@ -2747,11 +2747,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F49" s="1">
@@ -2795,12 +2795,12 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1333333333333333</v>
+        <f t="shared" si="11"/>
+        <v>0.22666666666666657</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="3"/>
@@ -2843,12 +2843,12 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333326</v>
+        <f t="shared" si="11"/>
+        <v>0.46666666666666679</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="3"/>
@@ -2891,11 +2891,11 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
@@ -2936,15 +2936,15 @@
         <v>0.2</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" ref="C53:C76" si="11">2/3</f>
+        <f t="shared" ref="C53:C76" si="12">2/3</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
@@ -2985,15 +2985,15 @@
         <v>0.6</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
@@ -3033,15 +3033,15 @@
         <v>0.8</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
@@ -3073,7 +3073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10</v>
       </c>
@@ -3081,16 +3081,16 @@
         <v>1</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>6.666666666666643E-2</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="3"/>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="H56" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="b">
         <f t="shared" si="6"/>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="L56" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -3129,15 +3129,15 @@
         <v>0</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
@@ -3178,15 +3178,15 @@
         <v>0.2</v>
       </c>
       <c r="C58" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
@@ -3227,15 +3227,15 @@
         <v>0.6</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
@@ -3267,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -3275,15 +3275,15 @@
         <v>0.8</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E60" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
@@ -3312,7 +3312,7 @@
       </c>
       <c r="L60" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -3323,16 +3323,16 @@
         <v>1</v>
       </c>
       <c r="C61" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="E61" s="1">
-        <f t="shared" si="2"/>
-        <v>0.16666666666666652</v>
+        <f t="shared" si="11"/>
+        <v>0.23333333333333339</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="3"/>
@@ -3371,15 +3371,15 @@
         <v>0</v>
       </c>
       <c r="C62" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E62" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
@@ -3420,15 +3420,15 @@
         <v>0.2</v>
       </c>
       <c r="C63" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E63" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
@@ -3460,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>20</v>
       </c>
@@ -3469,15 +3469,15 @@
         <v>0.6</v>
       </c>
       <c r="C64" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E64" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F64" s="1">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="L64" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -3517,16 +3517,16 @@
         <v>0.8</v>
       </c>
       <c r="C65" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E65" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1333333333333333</v>
+        <f t="shared" si="11"/>
+        <v>0.1599999999999997</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" si="3"/>
@@ -3565,16 +3565,16 @@
         <v>1</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E66" s="1">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333304</v>
+        <f t="shared" si="11"/>
+        <v>0.39999999999999991</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" si="3"/>
@@ -3597,7 +3597,7 @@
         <v>1</v>
       </c>
       <c r="K66" t="b">
-        <f t="shared" ref="K66:K101" si="12">IF(A66 &lt; 15, AND((B66 &gt;= 1),(C66 &gt;=2/3)), IF(A66 &lt; 30, AND((B66 &gt;= 2/3),(C66&gt;=1/2)),  AND((B66 &gt;= 1/3),(C66&gt;=1/5))))</f>
+        <f t="shared" ref="K66:K101" si="13">IF(A66 &lt; 15, AND((B66 &gt;= 1),(C66 &gt;=2/3)), IF(A66 &lt; 30, AND((B66 &gt;= 2/3),(C66&gt;=1/2)),  AND((B66 &gt;= 1/3),(C66&gt;=1/5))))</f>
         <v>1</v>
       </c>
       <c r="L66" t="b">
@@ -3613,15 +3613,15 @@
         <v>0</v>
       </c>
       <c r="C67" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D101" si="13">MIN(A67,30)/30</f>
+        <f t="shared" ref="D67:D101" si="14">MIN(A67,30)/30</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" ref="E67:E101" si="14">MAX(MAX(D67+B67 -1,0) + C67 - 1,0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F67" s="1">
@@ -3645,11 +3645,11 @@
         <v>0</v>
       </c>
       <c r="K67" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L67" t="b">
-        <f t="shared" ref="L67:L101" si="20">NOT(J67 = K67)</f>
+        <f t="shared" ref="L67:L101" si="20">NOT(H67 = K67)</f>
         <v>0</v>
       </c>
     </row>
@@ -3662,15 +3662,15 @@
         <v>0.2</v>
       </c>
       <c r="C68" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F68" s="1">
@@ -3694,7 +3694,7 @@
         <v>0</v>
       </c>
       <c r="K68" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L68" t="b">
@@ -3711,16 +3711,16 @@
         <v>0.6</v>
       </c>
       <c r="C69" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E69" s="1">
-        <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
+        <f t="shared" si="11"/>
+        <v>8.6666666666666448E-2</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" si="15"/>
@@ -3743,7 +3743,7 @@
         <v>1</v>
       </c>
       <c r="K69" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L69" t="b">
@@ -3759,16 +3759,16 @@
         <v>0.8</v>
       </c>
       <c r="C70" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="14"/>
-        <v>0.29999999999999982</v>
+        <f t="shared" si="11"/>
+        <v>0.32666666666666666</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" si="15"/>
@@ -3791,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="K70" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L70" t="b">
@@ -3807,16 +3807,16 @@
         <v>1</v>
       </c>
       <c r="C71" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D71">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" si="14"/>
-        <v>0.5</v>
+        <f t="shared" si="11"/>
+        <v>0.56666666666666643</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" si="15"/>
@@ -3839,7 +3839,7 @@
         <v>1</v>
       </c>
       <c r="K71" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L71" t="b">
@@ -3855,15 +3855,15 @@
         <v>0</v>
       </c>
       <c r="C72" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D72">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F72" s="1">
@@ -3887,7 +3887,7 @@
         <v>0</v>
       </c>
       <c r="K72" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L72" t="b">
@@ -3904,15 +3904,15 @@
         <v>0.2</v>
       </c>
       <c r="C73" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F73" s="1">
@@ -3936,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="K73" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L73" t="b">
@@ -3953,16 +3953,16 @@
         <v>0.6</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="14"/>
-        <v>0.26666666666666661</v>
+        <f t="shared" si="11"/>
+        <v>0.25333333333333341</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" si="15"/>
@@ -3985,7 +3985,7 @@
         <v>1</v>
       </c>
       <c r="K74" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L74" t="b">
@@ -4001,16 +4001,16 @@
         <v>0.8</v>
       </c>
       <c r="C75" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="14"/>
-        <v>0.46666666666666679</v>
+        <f t="shared" si="11"/>
+        <v>0.49333333333333318</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" si="15"/>
@@ -4033,7 +4033,7 @@
         <v>1</v>
       </c>
       <c r="K75" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L75" t="b">
@@ -4049,16 +4049,16 @@
         <v>1</v>
       </c>
       <c r="C76" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="14"/>
-        <v>0.66666666666666652</v>
+        <f t="shared" si="11"/>
+        <v>0.73333333333333339</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" si="15"/>
@@ -4081,7 +4081,7 @@
         <v>1</v>
       </c>
       <c r="K76" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L76" t="b">
@@ -4100,11 +4100,11 @@
         <v>1</v>
       </c>
       <c r="D77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F77" s="1">
@@ -4128,7 +4128,7 @@
         <v>0</v>
       </c>
       <c r="K77" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L77" t="b">
@@ -4148,11 +4148,11 @@
         <v>1</v>
       </c>
       <c r="D78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F78" s="1">
@@ -4176,7 +4176,7 @@
         <v>0</v>
       </c>
       <c r="K78" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L78" t="b">
@@ -4196,11 +4196,11 @@
         <v>1</v>
       </c>
       <c r="D79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F79" s="1">
@@ -4224,7 +4224,7 @@
         <v>0</v>
       </c>
       <c r="K79" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L79" t="b">
@@ -4243,12 +4243,12 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="14"/>
-        <v>0.1333333333333333</v>
+        <f t="shared" si="11"/>
+        <v>9.3333333333333268E-2</v>
       </c>
       <c r="F80" s="1">
         <f t="shared" si="15"/>
@@ -4271,7 +4271,7 @@
         <v>1</v>
       </c>
       <c r="K80" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L80" t="b">
@@ -4290,11 +4290,11 @@
         <v>1</v>
       </c>
       <c r="D81">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.33333333333333326</v>
       </c>
       <c r="F81" s="1">
@@ -4318,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="K81" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L81" t="b">
@@ -4337,11 +4337,11 @@
         <v>1</v>
       </c>
       <c r="D82">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="E82" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F82" s="1">
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="K82" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L82" t="b">
@@ -4385,11 +4385,11 @@
         <v>1</v>
       </c>
       <c r="D83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F83" s="1">
@@ -4413,7 +4413,7 @@
         <v>0</v>
       </c>
       <c r="K83" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L83" t="b">
@@ -4433,12 +4433,12 @@
         <v>1</v>
       </c>
       <c r="D84">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="E84" s="1">
-        <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
+        <f t="shared" si="11"/>
+        <v>2.0000000000000018E-2</v>
       </c>
       <c r="F84" s="1">
         <f t="shared" si="15"/>
@@ -4461,7 +4461,7 @@
         <v>1</v>
       </c>
       <c r="K84" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L84" t="b">
@@ -4480,12 +4480,12 @@
         <v>1</v>
       </c>
       <c r="D85">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="E85" s="1">
-        <f t="shared" si="14"/>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="11"/>
+        <v>0.26</v>
       </c>
       <c r="F85" s="1">
         <f t="shared" si="15"/>
@@ -4508,7 +4508,7 @@
         <v>1</v>
       </c>
       <c r="K85" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L85" t="b">
@@ -4527,11 +4527,11 @@
         <v>1</v>
       </c>
       <c r="D86">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="F86" s="1">
@@ -4555,7 +4555,7 @@
         <v>1</v>
       </c>
       <c r="K86" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L86" t="b">
@@ -4574,11 +4574,11 @@
         <v>1</v>
       </c>
       <c r="D87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E87" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F87" s="1">
@@ -4602,7 +4602,7 @@
         <v>0</v>
       </c>
       <c r="K87" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L87" t="b">
@@ -4622,11 +4622,11 @@
         <v>1</v>
       </c>
       <c r="D88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E88" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F88" s="1">
@@ -4650,7 +4650,7 @@
         <v>0</v>
       </c>
       <c r="K88" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L88" t="b">
@@ -4670,12 +4670,12 @@
         <v>1</v>
       </c>
       <c r="D89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E89" s="1">
-        <f t="shared" si="14"/>
-        <v>0.26666666666666661</v>
+        <f t="shared" si="11"/>
+        <v>0.18666666666666676</v>
       </c>
       <c r="F89" s="1">
         <f t="shared" si="15"/>
@@ -4698,7 +4698,7 @@
         <v>1</v>
       </c>
       <c r="K89" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L89" t="b">
@@ -4717,12 +4717,12 @@
         <v>1</v>
       </c>
       <c r="D90">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E90" s="1">
-        <f t="shared" si="14"/>
-        <v>0.46666666666666679</v>
+        <f t="shared" si="11"/>
+        <v>0.42666666666666653</v>
       </c>
       <c r="F90" s="1">
         <f t="shared" si="15"/>
@@ -4745,7 +4745,7 @@
         <v>1</v>
       </c>
       <c r="K90" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L90" t="b">
@@ -4764,12 +4764,12 @@
         <v>1</v>
       </c>
       <c r="D91">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E91" s="1">
-        <f t="shared" si="14"/>
-        <v>0.66666666666666652</v>
+        <f t="shared" si="11"/>
+        <v>0.66666666666666674</v>
       </c>
       <c r="F91" s="1">
         <f t="shared" si="15"/>
@@ -4792,7 +4792,7 @@
         <v>1</v>
       </c>
       <c r="K91" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L91" t="b">
@@ -4811,11 +4811,11 @@
         <v>1</v>
       </c>
       <c r="D92">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E92" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F92" s="1">
@@ -4839,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="K92" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L92" t="b">
@@ -4859,12 +4859,12 @@
         <v>1</v>
       </c>
       <c r="D93">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E93" s="1">
-        <f t="shared" si="14"/>
-        <v>3.3333333333333437E-2</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="F93" s="1">
         <f t="shared" si="15"/>
@@ -4876,7 +4876,7 @@
       </c>
       <c r="H93" t="b">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" t="b">
         <f t="shared" si="18"/>
@@ -4887,7 +4887,7 @@
         <v>0</v>
       </c>
       <c r="K93" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L93" t="b">
@@ -4907,12 +4907,12 @@
         <v>1</v>
       </c>
       <c r="D94">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E94" s="1">
-        <f t="shared" si="14"/>
-        <v>0.43333333333333335</v>
+        <f t="shared" si="11"/>
+        <v>0.35333333333333328</v>
       </c>
       <c r="F94" s="1">
         <f t="shared" si="15"/>
@@ -4935,7 +4935,7 @@
         <v>1</v>
       </c>
       <c r="K94" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L94" t="b">
@@ -4954,12 +4954,12 @@
         <v>1</v>
       </c>
       <c r="D95">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E95" s="1">
-        <f t="shared" si="14"/>
-        <v>0.6333333333333333</v>
+        <f t="shared" si="11"/>
+        <v>0.59333333333333349</v>
       </c>
       <c r="F95" s="1">
         <f t="shared" si="15"/>
@@ -4982,7 +4982,7 @@
         <v>1</v>
       </c>
       <c r="K95" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L95" t="b">
@@ -5001,12 +5001,12 @@
         <v>1</v>
       </c>
       <c r="D96">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="E96" s="1">
-        <f t="shared" si="14"/>
-        <v>0.83333333333333348</v>
+        <f t="shared" si="11"/>
+        <v>0.83333333333333326</v>
       </c>
       <c r="F96" s="1">
         <f t="shared" si="15"/>
@@ -5029,7 +5029,7 @@
         <v>1</v>
       </c>
       <c r="K96" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L96" t="b">
@@ -5048,11 +5048,11 @@
         <v>1</v>
       </c>
       <c r="D97">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E97" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F97" s="1">
@@ -5076,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="K97" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L97" t="b">
@@ -5084,7 +5084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>30</v>
       </c>
@@ -5096,12 +5096,12 @@
         <v>1</v>
       </c>
       <c r="D98">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E98" s="1">
-        <f t="shared" si="14"/>
-        <v>0.19999999999999996</v>
+        <f t="shared" si="11"/>
+        <v>4.0000000000000036E-2</v>
       </c>
       <c r="F98" s="1">
         <f t="shared" si="15"/>
@@ -5124,12 +5124,12 @@
         <v>0</v>
       </c>
       <c r="K98" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L98" t="b">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -5144,12 +5144,12 @@
         <v>1</v>
       </c>
       <c r="D99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E99" s="1">
-        <f t="shared" si="14"/>
-        <v>0.60000000000000009</v>
+        <f t="shared" si="11"/>
+        <v>0.52</v>
       </c>
       <c r="F99" s="1">
         <f t="shared" si="15"/>
@@ -5172,7 +5172,7 @@
         <v>1</v>
       </c>
       <c r="K99" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L99" t="b">
@@ -5191,12 +5191,12 @@
         <v>1</v>
       </c>
       <c r="D100">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E100" s="1">
-        <f t="shared" si="14"/>
-        <v>0.8</v>
+        <f t="shared" si="11"/>
+        <v>0.76</v>
       </c>
       <c r="F100" s="1">
         <f t="shared" si="15"/>
@@ -5219,7 +5219,7 @@
         <v>1</v>
       </c>
       <c r="K100" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L100" t="b">
@@ -5238,11 +5238,11 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E101" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="F101" s="1">
@@ -5266,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="K101" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L101" t="b">

</xml_diff>